<commit_message>
dr and dr_idv added to the uncertainty analysis
</commit_message>
<xml_diff>
--- a/Interface_RDM.xlsx
+++ b/Interface_RDM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rdm_kenya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E283180A-7017-4519-A75B-C4F853BCFB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C572DF5-3389-415C-A98D-A48307B243C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="460" activeTab="1" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="3" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="177">
   <si>
     <t>X_Num</t>
   </si>
@@ -595,6 +595,18 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Discount rate</t>
+  </si>
+  <si>
+    <t>Global discount rate</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Technology specific discount rate</t>
   </si>
 </sst>
 </file>
@@ -953,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1056,6 +1068,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1380,7 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EBD12E-40AD-42BC-9E38-C5D5CF6C4FA5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1461,8 +1474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,181 +2064,443 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+    <row r="15" spans="1:15" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="27">
+        <v>14</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H15" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="28">
+        <v>1.5</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>41</v>
+      </c>
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
       <c r="M15" s="28"/>
-      <c r="N15" s="31"/>
-    </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="29"/>
+      <c r="N15" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <v>15</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H16" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="I16" s="28">
+        <v>1.3</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="L16" s="29"/>
       <c r="M16" s="28"/>
-      <c r="N16" s="31"/>
-    </row>
-    <row r="17" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
+      <c r="N16" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <v>16</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H17" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="I17" s="28">
+        <v>1.4</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>160</v>
+      </c>
       <c r="L17" s="29"/>
       <c r="M17" s="28"/>
-      <c r="N17" s="31"/>
-    </row>
-    <row r="18" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="29"/>
+      <c r="N17" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>17</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H18" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="I18" s="28">
+        <v>1.4</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>161</v>
+      </c>
       <c r="L18" s="29"/>
       <c r="M18" s="28"/>
-      <c r="N18" s="31"/>
-    </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="29"/>
+      <c r="N18" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <v>18</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H19" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="I19" s="28">
+        <v>1.3</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>162</v>
+      </c>
       <c r="L19" s="29"/>
       <c r="M19" s="28"/>
-      <c r="N19" s="31"/>
-    </row>
-    <row r="20" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
+      <c r="N19" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
+        <v>19</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H20" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="I20" s="28">
+        <v>1.4</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>163</v>
+      </c>
       <c r="L20" s="29"/>
       <c r="M20" s="28"/>
-      <c r="N20" s="31"/>
-    </row>
-    <row r="21" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="29"/>
+      <c r="N20" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="27">
+        <v>20</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H21" s="28">
+        <v>0</v>
+      </c>
+      <c r="I21" s="28">
+        <v>2</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="L21" s="29"/>
       <c r="M21" s="28"/>
-      <c r="N21" s="31"/>
-    </row>
-    <row r="22" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="29"/>
+      <c r="N21" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="27">
+        <v>21</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H22" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="I22" s="28">
+        <v>1.25</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>165</v>
+      </c>
       <c r="L22" s="29"/>
       <c r="M22" s="28"/>
-      <c r="N22" s="31"/>
-    </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="29"/>
+      <c r="N22" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="27">
+        <v>22</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H23" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="28">
+        <v>1.5</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>166</v>
+      </c>
       <c r="L23" s="29"/>
       <c r="M23" s="28"/>
-      <c r="N23" s="31"/>
-    </row>
-    <row r="24" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="29"/>
+      <c r="N23" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="27">
+        <v>23</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H24" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="I24" s="28">
+        <v>1.3</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K24" s="29" t="s">
+        <v>167</v>
+      </c>
       <c r="L24" s="29"/>
       <c r="M24" s="28"/>
-      <c r="N24" s="31"/>
-    </row>
-    <row r="25" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="29"/>
+      <c r="N24" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="27">
+        <v>24</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="28">
+        <v>2025</v>
+      </c>
+      <c r="H25" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="I25" s="28">
+        <v>1.3</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>168</v>
+      </c>
       <c r="L25" s="29"/>
       <c r="M25" s="28"/>
-      <c r="N25" s="31"/>
+      <c r="N25" s="22" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2488,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7095350F-2181-46D9-957F-C928CA3CEF59}">
   <dimension ref="A1:BG5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,10 +2833,10 @@
       <c r="B1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="40" t="s">
         <v>114</v>
       </c>
       <c r="E1" s="36" t="s">
@@ -2738,11 +3013,10 @@
         <f t="shared" ref="B2:AQ2" si="0">+COUNTA(B3:B1048576)</f>
         <v>1</v>
       </c>
-      <c r="C2" s="36">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D2" s="36">
+      <c r="C2" s="40">
+        <v>0</v>
+      </c>
+      <c r="D2" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2971,11 +3245,9 @@
       <c r="B3" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>128</v>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40" t="s">
+        <v>132</v>
       </c>
       <c r="E3" s="36" t="s">
         <v>128</v>
@@ -3144,8 +3416,8 @@
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
@@ -3220,8 +3492,8 @@
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>

</xml_diff>